<commit_message>
Add script to edit mm in tts
Script edits mm info in tts:
-add vp tag
-add card name
-sync image files with shiny app images

also fix data bug with onslaught epic
</commit_message>
<xml_diff>
--- a/data/masterminds.xlsx
+++ b/data/masterminds.xlsx
@@ -3699,10 +3699,10 @@
   <dimension ref="A1:AA404"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="R373" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B156" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AA401" sqref="AA401:AA404"/>
+      <selection pane="bottomRight" activeCell="C148" sqref="C148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7567,9 +7567,6 @@
       <c r="B148" t="s">
         <v>137</v>
       </c>
-      <c r="C148">
-        <v>1</v>
-      </c>
       <c r="E148" t="s">
         <v>32</v>
       </c>

</xml_diff>

<commit_message>
split cards, mastermind fight
Sort out split and multiclass cards
Fix scripts to support them
Adjust hasTag2 and stop its proliferation

Try to do unveiled schemes

Make mastermind power buttons and fight scripting work like villains in city
</commit_message>
<xml_diff>
--- a/data/masterminds.xlsx
+++ b/data/masterminds.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2772" uniqueCount="1185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2771" uniqueCount="1184">
   <si>
     <t>Name</t>
   </si>
@@ -3489,9 +3489,6 @@
   </si>
   <si>
     <t>Purifiers</t>
-  </si>
-  <si>
-    <t>Sentinel</t>
   </si>
   <si>
     <t>6</t>
@@ -3921,10 +3918,10 @@
   <dimension ref="A1:AA446"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="X416" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B409" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AA447" sqref="AA447"/>
+      <selection pane="bottomRight" activeCell="G431" sqref="G431"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10814,6 +10811,12 @@
       <c r="E270" t="s">
         <v>208</v>
       </c>
+      <c r="H270">
+        <v>6</v>
+      </c>
+      <c r="I270" s="7" t="s">
+        <v>1123</v>
+      </c>
       <c r="T270">
         <v>1</v>
       </c>
@@ -14760,9 +14763,6 @@
       <c r="F429" t="s">
         <v>1157</v>
       </c>
-      <c r="G429" t="s">
-        <v>1158</v>
-      </c>
       <c r="H429">
         <v>6</v>
       </c>
@@ -14773,7 +14773,7 @@
         <v>1</v>
       </c>
       <c r="Z429" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
       <c r="AA429">
         <v>1</v>
@@ -14792,14 +14792,11 @@
       <c r="F430" t="s">
         <v>1157</v>
       </c>
-      <c r="G430" t="s">
-        <v>1158</v>
-      </c>
       <c r="H430">
         <v>6</v>
       </c>
       <c r="I430" s="7" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
       <c r="R430">
         <v>1</v>
@@ -14808,7 +14805,7 @@
         <v>1</v>
       </c>
       <c r="Z430" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
       <c r="AA430">
         <v>1</v>
@@ -14816,7 +14813,7 @@
     </row>
     <row r="431" spans="1:27">
       <c r="A431" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
       <c r="B431" t="s">
         <v>1156</v>
@@ -14833,7 +14830,7 @@
     </row>
     <row r="432" spans="1:27">
       <c r="A432" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="B432" t="s">
         <v>1156</v>
@@ -14850,7 +14847,7 @@
     </row>
     <row r="433" spans="1:27">
       <c r="A433" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="B433" t="s">
         <v>1156</v>
@@ -14867,7 +14864,7 @@
     </row>
     <row r="434" spans="1:27">
       <c r="A434" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
       <c r="B434" t="s">
         <v>1156</v>
@@ -14884,25 +14881,25 @@
     </row>
     <row r="435" spans="1:27">
       <c r="A435" t="s">
+        <v>1165</v>
+      </c>
+      <c r="E435" t="s">
         <v>1166</v>
       </c>
-      <c r="E435" t="s">
+      <c r="F435" t="s">
         <v>1167</v>
-      </c>
-      <c r="F435" t="s">
-        <v>1168</v>
       </c>
       <c r="H435">
         <v>6</v>
       </c>
       <c r="I435" s="7" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
       <c r="R435">
         <v>1</v>
       </c>
       <c r="Z435" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
       <c r="AA435">
         <v>1</v>
@@ -14910,16 +14907,16 @@
     </row>
     <row r="436" spans="1:27">
       <c r="A436" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C436">
+        <v>1</v>
+      </c>
+      <c r="E436" t="s">
         <v>1166</v>
       </c>
-      <c r="C436">
-        <v>1</v>
-      </c>
-      <c r="E436" t="s">
+      <c r="F436" t="s">
         <v>1167</v>
-      </c>
-      <c r="F436" t="s">
-        <v>1168</v>
       </c>
       <c r="H436">
         <v>6</v>
@@ -14931,7 +14928,7 @@
         <v>1</v>
       </c>
       <c r="Z436" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
       <c r="AA436">
         <v>1</v>
@@ -14939,16 +14936,16 @@
     </row>
     <row r="437" spans="1:27">
       <c r="A437" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
       <c r="B437" t="s">
+        <v>1165</v>
+      </c>
+      <c r="E437" t="s">
         <v>1166</v>
       </c>
-      <c r="E437" t="s">
-        <v>1167</v>
-      </c>
       <c r="Z437" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
       <c r="AA437" t="s">
         <v>999</v>
@@ -14956,16 +14953,16 @@
     </row>
     <row r="438" spans="1:27">
       <c r="A438" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
       <c r="B438" t="s">
+        <v>1165</v>
+      </c>
+      <c r="E438" t="s">
         <v>1166</v>
       </c>
-      <c r="E438" t="s">
-        <v>1167</v>
-      </c>
       <c r="Z438" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
       <c r="AA438" t="s">
         <v>1000</v>
@@ -14973,16 +14970,16 @@
     </row>
     <row r="439" spans="1:27">
       <c r="A439" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
       <c r="B439" t="s">
+        <v>1165</v>
+      </c>
+      <c r="E439" t="s">
         <v>1166</v>
       </c>
-      <c r="E439" t="s">
-        <v>1167</v>
-      </c>
       <c r="Z439" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
       <c r="AA439" t="s">
         <v>1001</v>
@@ -14990,16 +14987,16 @@
     </row>
     <row r="440" spans="1:27">
       <c r="A440" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
       <c r="B440" t="s">
+        <v>1165</v>
+      </c>
+      <c r="E440" t="s">
         <v>1166</v>
       </c>
-      <c r="E440" t="s">
-        <v>1167</v>
-      </c>
       <c r="Z440" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
       <c r="AA440" t="s">
         <v>1005</v>
@@ -15007,13 +15004,13 @@
     </row>
     <row r="441" spans="1:27">
       <c r="A441" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
       <c r="E441" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
       <c r="F441" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="H441">
         <v>6</v>
@@ -15022,7 +15019,7 @@
         <v>1153</v>
       </c>
       <c r="Z441" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
       <c r="AA441">
         <v>1</v>
@@ -15030,25 +15027,25 @@
     </row>
     <row r="442" spans="1:27">
       <c r="A442" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
       <c r="C442">
         <v>1</v>
       </c>
       <c r="E442" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
       <c r="F442" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="H442">
         <v>6</v>
       </c>
       <c r="I442" s="7" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
       <c r="Z442" t="s">
-        <v>1184</v>
+        <v>1183</v>
       </c>
       <c r="AA442">
         <v>1</v>
@@ -15056,16 +15053,16 @@
     </row>
     <row r="443" spans="1:27">
       <c r="A443" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="B443" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
       <c r="E443" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
       <c r="Z443" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
       <c r="AA443" t="s">
         <v>1009</v>
@@ -15073,16 +15070,16 @@
     </row>
     <row r="444" spans="1:27">
       <c r="A444" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
       <c r="B444" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
       <c r="E444" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
       <c r="Z444" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
       <c r="AA444" t="s">
         <v>981</v>
@@ -15090,16 +15087,16 @@
     </row>
     <row r="445" spans="1:27">
       <c r="A445" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
       <c r="B445" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
       <c r="E445" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
       <c r="Z445" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
       <c r="AA445" t="s">
         <v>985</v>
@@ -15107,16 +15104,16 @@
     </row>
     <row r="446" spans="1:27">
       <c r="A446" t="s">
-        <v>1182</v>
+        <v>1181</v>
       </c>
       <c r="B446" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
       <c r="E446" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
       <c r="Z446" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
       <c r="AA446" t="s">
         <v>988</v>

</xml_diff>